<commit_message>
drop row/column if every cell in it is empty
</commit_message>
<xml_diff>
--- a/champions.xlsx
+++ b/champions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\5dars\PycharmProjects\Data Cleaning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EAC8863-B9BF-4AF7-906C-DECE388A44F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B8C240-61DC-44F0-A9F1-9BEE1FAC8114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A8605B52-9432-49E7-A343-C706373D400E}"/>
   </bookViews>
@@ -1363,3475 +1363,3476 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{596795FE-1D32-459C-BE44-8C2C7F5063E2}">
-  <dimension ref="A1:G151"/>
+  <dimension ref="A1:H151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.08984375" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>160</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>158</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>580</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>38</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>60</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>1.05</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>580</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>38</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>60</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>1.05</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>526</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>418</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>21</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>53</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>1.02</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>575</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>200</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>23</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>600</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>350</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>62</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>1.08</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>285</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>33</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>53</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>1.06</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>480</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>21</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>51</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>1.01</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>524</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>418</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>19</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>50</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>570</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>280</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>26</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>1.04</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>575</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>350</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>19</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>57</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>1.02</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>18</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>552</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>438</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>19</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>52</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>1.01</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>560</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>350</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>34</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>52</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>1.05</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>20</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>583</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>267</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>37</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>61</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>1.07</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>21</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>590</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>469</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>22</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>57</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>1.03</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>22</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>540</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>311</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>47</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>55</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>1.06</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>23</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>510</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>313</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>28</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>62</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>1.05</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>24</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>576</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>339</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>35</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>68</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>1.06</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>25</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>560</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>800</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>18</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>53</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>1.02</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>26</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>574</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>272</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>38</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>69</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>1.08</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>27</v>
       </c>
       <c r="B21" t="s">
         <v>16</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>518</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>350</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>28</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>55</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>1.04</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>28</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>582</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>263</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>39</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>64</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>1.07</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>29</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>570</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>375</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>31</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>57</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>1.03</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>30</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>582</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>0</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>36</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>61</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>1.06</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>31</v>
       </c>
       <c r="B25" t="s">
         <v>16</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>574</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>360</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>29</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>61</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>1.05</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>32</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>585</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>280</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>32</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>58</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>1.03</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>33</v>
       </c>
       <c r="B27" t="s">
         <v>12</v>
       </c>
-      <c r="C27">
+      <c r="D27">
         <v>529</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>324</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>27</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>55</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>1.03</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>34</v>
       </c>
       <c r="B28" t="s">
         <v>12</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>572</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>315</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>37</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>61</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>1.05</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>35</v>
       </c>
       <c r="B29" t="s">
         <v>16</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <v>530</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>375</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>22</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>60</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>1.04</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>36</v>
       </c>
       <c r="B30" t="s">
         <v>12</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <v>580</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>500</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>34</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>55</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>1.04</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>37</v>
       </c>
       <c r="B31" t="s">
         <v>5</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <v>550</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>300</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>33</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>68</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>1.06</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>38</v>
       </c>
       <c r="B32" t="s">
         <v>7</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <v>570</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>317</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>22</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>58</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>1.03</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>39</v>
       </c>
       <c r="B33" t="s">
         <v>7</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <v>562</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>500</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>24</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>59</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>1.04</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>40</v>
       </c>
       <c r="B34" t="s">
         <v>5</v>
       </c>
-      <c r="C34">
+      <c r="D34">
         <v>540</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>280</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>35</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>64</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>1.05</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>41</v>
       </c>
       <c r="B35" t="s">
         <v>5</v>
       </c>
-      <c r="C35">
+      <c r="D35">
         <v>620</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>0</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>36</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>66</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <v>1.07</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>42</v>
       </c>
       <c r="B36" t="s">
         <v>5</v>
       </c>
-      <c r="C36">
+      <c r="D36">
         <v>510</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>100</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>32</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>59</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>1.03</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>43</v>
       </c>
       <c r="B37" t="s">
         <v>12</v>
       </c>
-      <c r="C37">
+      <c r="D37">
         <v>600</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>400</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>38</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>64</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>1.07</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>44</v>
       </c>
       <c r="B38" t="s">
         <v>12</v>
       </c>
-      <c r="C38">
+      <c r="D38">
         <v>555</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>322</v>
       </c>
-      <c r="E38">
+      <c r="F38">
         <v>33</v>
       </c>
-      <c r="F38">
+      <c r="G38">
         <v>66</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <v>1.05</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>45</v>
       </c>
       <c r="B39" t="s">
         <v>12</v>
       </c>
-      <c r="C39">
+      <c r="D39">
         <v>580</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>277</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>36</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>66</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>1.06</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>46</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
       </c>
-      <c r="C40">
+      <c r="D40">
         <v>488</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>385</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>19</v>
       </c>
-      <c r="F40">
+      <c r="G40">
         <v>55</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>1.01</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>47</v>
       </c>
       <c r="B41" t="s">
         <v>5</v>
       </c>
-      <c r="C41">
+      <c r="D41">
         <v>585</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <v>300</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>35</v>
       </c>
-      <c r="F41">
+      <c r="G41">
         <v>68</v>
       </c>
-      <c r="G41">
+      <c r="H41">
         <v>1.06</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>48</v>
       </c>
       <c r="B42" t="s">
         <v>5</v>
       </c>
-      <c r="C42">
+      <c r="D42">
         <v>590</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>350</v>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>36</v>
       </c>
-      <c r="F42">
+      <c r="G42">
         <v>63</v>
       </c>
-      <c r="G42">
+      <c r="H42">
         <v>1.06</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>49</v>
       </c>
       <c r="B43" t="s">
         <v>12</v>
       </c>
-      <c r="C43">
+      <c r="D43">
         <v>585</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <v>450</v>
       </c>
-      <c r="E43">
+      <c r="F43">
         <v>27</v>
       </c>
-      <c r="F43">
+      <c r="G43">
         <v>50</v>
       </c>
-      <c r="G43">
+      <c r="H43">
         <v>1.03</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>50</v>
       </c>
       <c r="B44" t="s">
         <v>10</v>
       </c>
-      <c r="C44">
+      <c r="D44">
         <v>500</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>350</v>
       </c>
-      <c r="E44">
+      <c r="F44">
         <v>28</v>
       </c>
-      <c r="F44">
+      <c r="G44">
         <v>46</v>
       </c>
-      <c r="G44">
+      <c r="H44">
         <v>1.02</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>51</v>
       </c>
       <c r="B45" t="s">
         <v>12</v>
       </c>
-      <c r="C45">
+      <c r="D45">
         <v>570</v>
       </c>
-      <c r="D45">
+      <c r="E45">
         <v>300</v>
       </c>
-      <c r="E45">
+      <c r="F45">
         <v>34</v>
       </c>
-      <c r="F45">
+      <c r="G45">
         <v>64</v>
       </c>
-      <c r="G45">
+      <c r="H45">
         <v>1.05</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>52</v>
       </c>
       <c r="B46" t="s">
         <v>5</v>
       </c>
-      <c r="C46">
+      <c r="D46">
         <v>592</v>
       </c>
-      <c r="D46">
+      <c r="E46">
         <v>338</v>
       </c>
-      <c r="E46">
+      <c r="F46">
         <v>36</v>
       </c>
-      <c r="F46">
+      <c r="G46">
         <v>68</v>
       </c>
-      <c r="G46">
+      <c r="H46">
         <v>1.07</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>53</v>
       </c>
       <c r="B47" t="s">
         <v>5</v>
       </c>
-      <c r="C47">
+      <c r="D47">
         <v>560</v>
       </c>
-      <c r="D47">
+      <c r="E47">
         <v>375</v>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>22</v>
       </c>
-      <c r="F47">
+      <c r="G47">
         <v>54</v>
       </c>
-      <c r="G47">
+      <c r="H47">
         <v>1.02</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>54</v>
       </c>
       <c r="B48" t="s">
         <v>16</v>
       </c>
-      <c r="C48">
+      <c r="D48">
         <v>585</v>
       </c>
-      <c r="D48">
+      <c r="E48">
         <v>300</v>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>24</v>
       </c>
-      <c r="F48">
+      <c r="G48">
         <v>59</v>
       </c>
-      <c r="G48">
+      <c r="H48">
         <v>1.05</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>55</v>
       </c>
       <c r="B49" t="s">
         <v>16</v>
       </c>
-      <c r="C49">
+      <c r="D49">
         <v>550</v>
       </c>
-      <c r="D49">
+      <c r="E49">
         <v>245</v>
       </c>
-      <c r="E49">
+      <c r="F49">
         <v>28</v>
       </c>
-      <c r="F49">
+      <c r="G49">
         <v>57</v>
       </c>
-      <c r="G49">
+      <c r="H49">
         <v>1.04</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>56</v>
       </c>
       <c r="B50" t="s">
         <v>16</v>
       </c>
-      <c r="C50">
+      <c r="D50">
         <v>600</v>
       </c>
-      <c r="D50">
+      <c r="E50">
         <v>344</v>
       </c>
-      <c r="E50">
+      <c r="F50">
         <v>33</v>
       </c>
-      <c r="F50">
+      <c r="G50">
         <v>62</v>
       </c>
-      <c r="G50">
+      <c r="H50">
         <v>1.06</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>57</v>
       </c>
       <c r="B51" t="s">
         <v>16</v>
       </c>
-      <c r="C51">
+      <c r="D51">
         <v>534</v>
       </c>
-      <c r="D51">
+      <c r="E51">
         <v>250</v>
       </c>
-      <c r="E51">
+      <c r="F51">
         <v>21</v>
       </c>
-      <c r="F51">
+      <c r="G51">
         <v>69</v>
       </c>
-      <c r="G51">
+      <c r="H51">
         <v>1.05</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>58</v>
       </c>
       <c r="B52" t="s">
         <v>10</v>
       </c>
-      <c r="C52">
+      <c r="D52">
         <v>534</v>
       </c>
-      <c r="D52">
+      <c r="E52">
         <v>374</v>
       </c>
-      <c r="E52">
+      <c r="F52">
         <v>26</v>
       </c>
-      <c r="F52">
+      <c r="G52">
         <v>53</v>
       </c>
-      <c r="G52">
+      <c r="H52">
         <v>1.03</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>59</v>
       </c>
       <c r="B53" t="s">
         <v>12</v>
       </c>
-      <c r="C53">
+      <c r="D53">
         <v>528</v>
       </c>
-      <c r="D53">
+      <c r="E53">
         <v>467</v>
       </c>
-      <c r="E53">
+      <c r="F53">
         <v>21</v>
       </c>
-      <c r="F53">
+      <c r="G53">
         <v>45</v>
       </c>
-      <c r="G53">
+      <c r="H53">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>60</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
       </c>
-      <c r="C54">
+      <c r="D54">
         <v>576</v>
       </c>
-      <c r="D54">
+      <c r="E54">
         <v>400</v>
       </c>
-      <c r="E54">
+      <c r="F54">
         <v>19</v>
       </c>
-      <c r="F54">
+      <c r="G54">
         <v>59</v>
       </c>
-      <c r="G54">
+      <c r="H54">
         <v>1.02</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>61</v>
       </c>
       <c r="B55" t="s">
         <v>7</v>
       </c>
-      <c r="C55">
+      <c r="D55">
         <v>602</v>
       </c>
-      <c r="D55">
+      <c r="E55">
         <v>0</v>
       </c>
-      <c r="E55">
+      <c r="F55">
         <v>27</v>
       </c>
-      <c r="F55">
+      <c r="G55">
         <v>58</v>
       </c>
-      <c r="G55">
+      <c r="H55">
         <v>1.04</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>62</v>
       </c>
       <c r="B56" t="s">
         <v>5</v>
       </c>
-      <c r="C56">
+      <c r="D56">
         <v>600</v>
       </c>
-      <c r="D56">
+      <c r="E56">
         <v>330</v>
       </c>
-      <c r="E56">
+      <c r="F56">
         <v>26</v>
       </c>
-      <c r="F56">
+      <c r="G56">
         <v>50</v>
       </c>
-      <c r="G56">
+      <c r="H56">
         <v>1.02</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>63</v>
       </c>
       <c r="B57" t="s">
         <v>12</v>
       </c>
-      <c r="C57">
+      <c r="D57">
         <v>585</v>
       </c>
-      <c r="D57">
+      <c r="E57">
         <v>410</v>
       </c>
-      <c r="E57">
+      <c r="F57">
         <v>38</v>
       </c>
-      <c r="F57">
+      <c r="G57">
         <v>68</v>
       </c>
-      <c r="G57">
+      <c r="H57">
         <v>1.07</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>64</v>
       </c>
       <c r="B58" t="s">
         <v>5</v>
       </c>
-      <c r="C58">
+      <c r="D58">
         <v>541</v>
       </c>
-      <c r="D58">
+      <c r="E58">
         <v>200</v>
       </c>
-      <c r="E58">
+      <c r="F58">
         <v>29</v>
       </c>
-      <c r="F58">
+      <c r="G58">
         <v>48</v>
       </c>
-      <c r="G58">
+      <c r="H58">
         <v>1.01</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>65</v>
       </c>
       <c r="B59" t="s">
         <v>12</v>
       </c>
-      <c r="C59">
+      <c r="D59">
         <v>573</v>
       </c>
-      <c r="D59">
+      <c r="E59">
         <v>327</v>
       </c>
-      <c r="E59">
+      <c r="F59">
         <v>36</v>
       </c>
-      <c r="F59">
+      <c r="G59">
         <v>63</v>
       </c>
-      <c r="G59">
+      <c r="H59">
         <v>1.05</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>66</v>
       </c>
       <c r="B60" t="s">
         <v>12</v>
       </c>
-      <c r="C60">
+      <c r="D60">
         <v>540</v>
       </c>
-      <c r="D60">
+      <c r="E60">
         <v>300</v>
       </c>
-      <c r="E60">
+      <c r="F60">
         <v>29</v>
       </c>
-      <c r="F60">
+      <c r="G60">
         <v>65</v>
       </c>
-      <c r="G60">
+      <c r="H60">
         <v>1.05</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>67</v>
       </c>
       <c r="B61" t="s">
         <v>5</v>
       </c>
-      <c r="C61">
+      <c r="D61">
         <v>340</v>
       </c>
-      <c r="D61">
+      <c r="E61">
         <v>100</v>
       </c>
-      <c r="E61">
+      <c r="F61">
         <v>35</v>
       </c>
-      <c r="F61">
+      <c r="G61">
         <v>65</v>
       </c>
-      <c r="G61">
+      <c r="H61">
         <v>1.04</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>68</v>
       </c>
       <c r="B62" t="s">
         <v>16</v>
       </c>
-      <c r="C62">
+      <c r="D62">
         <v>534</v>
       </c>
-      <c r="D62">
+      <c r="E62">
         <v>325</v>
       </c>
-      <c r="E62">
+      <c r="F62">
         <v>24</v>
       </c>
-      <c r="F62">
+      <c r="G62">
         <v>57</v>
       </c>
-      <c r="G62">
+      <c r="H62">
         <v>1.03</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>69</v>
       </c>
       <c r="B63" t="s">
         <v>7</v>
       </c>
-      <c r="C63">
+      <c r="D63">
         <v>528</v>
       </c>
-      <c r="D63">
+      <c r="E63">
         <v>334</v>
       </c>
-      <c r="E63">
+      <c r="F63">
         <v>22</v>
       </c>
-      <c r="F63">
+      <c r="G63">
         <v>55</v>
       </c>
-      <c r="G63">
+      <c r="H63">
         <v>1.02</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>70</v>
       </c>
       <c r="B64" t="s">
         <v>12</v>
       </c>
-      <c r="C64">
+      <c r="D64">
         <v>575</v>
       </c>
-      <c r="D64">
+      <c r="E64">
         <v>200</v>
       </c>
-      <c r="E64">
+      <c r="F64">
         <v>33</v>
       </c>
-      <c r="F64">
+      <c r="G64">
         <v>70</v>
       </c>
-      <c r="G64">
+      <c r="H64">
         <v>1.07</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>71</v>
       </c>
       <c r="B65" t="s">
         <v>10</v>
       </c>
-      <c r="C65">
+      <c r="D65">
         <v>576</v>
       </c>
-      <c r="D65">
+      <c r="E65">
         <v>302</v>
       </c>
-      <c r="E65">
+      <c r="F65">
         <v>47</v>
       </c>
-      <c r="F65">
+      <c r="G65">
         <v>60</v>
       </c>
-      <c r="G65">
+      <c r="H65">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>72</v>
       </c>
       <c r="B66" t="s">
         <v>7</v>
       </c>
-      <c r="C66">
+      <c r="D66">
         <v>550</v>
       </c>
-      <c r="D66">
+      <c r="E66">
         <v>475</v>
       </c>
-      <c r="E66">
+      <c r="F66">
         <v>22</v>
       </c>
-      <c r="F66">
+      <c r="G66">
         <v>53</v>
       </c>
-      <c r="G66">
+      <c r="H66">
         <v>1.02</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>73</v>
       </c>
       <c r="B67" t="s">
         <v>16</v>
       </c>
-      <c r="C67">
+      <c r="D67">
         <v>571</v>
       </c>
-      <c r="D67">
+      <c r="E67">
         <v>348</v>
       </c>
-      <c r="E67">
+      <c r="F67">
         <v>28</v>
       </c>
-      <c r="F67">
+      <c r="G67">
         <v>64</v>
       </c>
-      <c r="G67">
+      <c r="H67">
         <v>1.05</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>74</v>
       </c>
       <c r="B68" t="s">
         <v>10</v>
       </c>
-      <c r="C68">
+      <c r="D68">
         <v>525</v>
       </c>
-      <c r="D68">
+      <c r="E68">
         <v>350</v>
       </c>
-      <c r="E68">
+      <c r="F68">
         <v>29</v>
       </c>
-      <c r="F68">
+      <c r="G68">
         <v>47</v>
       </c>
-      <c r="G68">
+      <c r="H68">
         <v>1.02</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>75</v>
       </c>
       <c r="B69" t="s">
         <v>7</v>
       </c>
-      <c r="C69">
+      <c r="D69">
         <v>490</v>
       </c>
-      <c r="D69">
+      <c r="E69">
         <v>480</v>
       </c>
-      <c r="E69">
+      <c r="F69">
         <v>18</v>
       </c>
-      <c r="F69">
+      <c r="G69">
         <v>54</v>
       </c>
-      <c r="G69">
+      <c r="H69">
         <v>1.01</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>76</v>
       </c>
       <c r="B70" t="s">
         <v>5</v>
       </c>
-      <c r="C70">
+      <c r="D70">
         <v>574</v>
       </c>
-      <c r="D70">
+      <c r="E70">
         <v>280</v>
       </c>
-      <c r="E70">
+      <c r="F70">
         <v>37</v>
       </c>
-      <c r="F70">
+      <c r="G70">
         <v>62</v>
       </c>
-      <c r="G70">
+      <c r="H70">
         <v>1.05</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>77</v>
       </c>
       <c r="B71" t="s">
         <v>7</v>
       </c>
-      <c r="C71">
+      <c r="D71">
         <v>510</v>
       </c>
-      <c r="D71">
+      <c r="E71">
         <v>375</v>
       </c>
-      <c r="E71">
+      <c r="F71">
         <v>18</v>
       </c>
-      <c r="F71">
+      <c r="G71">
         <v>55</v>
       </c>
-      <c r="G71">
+      <c r="H71">
         <v>1.01</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>78</v>
       </c>
       <c r="B72" t="s">
         <v>5</v>
       </c>
-      <c r="C72">
+      <c r="D72">
         <v>565</v>
       </c>
-      <c r="D72">
+      <c r="E72">
         <v>375</v>
       </c>
-      <c r="E72">
+      <c r="F72">
         <v>39</v>
       </c>
-      <c r="F72">
+      <c r="G72">
         <v>64</v>
       </c>
-      <c r="G72">
+      <c r="H72">
         <v>1.07</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>79</v>
       </c>
       <c r="B73" t="s">
         <v>12</v>
       </c>
-      <c r="C73">
+      <c r="D73">
         <v>598</v>
       </c>
-      <c r="D73">
+      <c r="E73">
         <v>250</v>
       </c>
-      <c r="E73">
+      <c r="F73">
         <v>33</v>
       </c>
-      <c r="F73">
+      <c r="G73">
         <v>66</v>
       </c>
-      <c r="G73">
+      <c r="H73">
         <v>1.06</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>80</v>
       </c>
       <c r="B74" t="s">
         <v>16</v>
       </c>
-      <c r="C74">
+      <c r="D74">
         <v>570</v>
       </c>
-      <c r="D74">
+      <c r="E74">
         <v>300</v>
       </c>
-      <c r="E74">
+      <c r="F74">
         <v>28</v>
       </c>
-      <c r="F74">
+      <c r="G74">
         <v>52</v>
       </c>
-      <c r="G74">
+      <c r="H74">
         <v>1.02</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>81</v>
       </c>
       <c r="B75" t="s">
         <v>5</v>
       </c>
-      <c r="C75">
+      <c r="D75">
         <v>575</v>
       </c>
-      <c r="D75">
+      <c r="E75">
         <v>0</v>
       </c>
-      <c r="E75">
+      <c r="F75">
         <v>37</v>
       </c>
-      <c r="F75">
+      <c r="G75">
         <v>61</v>
       </c>
-      <c r="G75">
+      <c r="H75">
         <v>1.06</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>82</v>
       </c>
       <c r="B76" t="s">
         <v>10</v>
       </c>
-      <c r="C76">
+      <c r="D76">
         <v>560</v>
       </c>
-      <c r="D76">
+      <c r="E76">
         <v>340</v>
       </c>
-      <c r="E76">
+      <c r="F76">
         <v>25</v>
       </c>
-      <c r="F76">
+      <c r="G76">
         <v>56</v>
       </c>
-      <c r="G76">
+      <c r="H76">
         <v>1.03</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>83</v>
       </c>
       <c r="B77" t="s">
         <v>10</v>
       </c>
-      <c r="C77">
+      <c r="D77">
         <v>475</v>
       </c>
-      <c r="D77">
+      <c r="E77">
         <v>365</v>
       </c>
-      <c r="E77">
+      <c r="F77">
         <v>29</v>
       </c>
-      <c r="F77">
+      <c r="G77">
         <v>51</v>
       </c>
-      <c r="G77">
+      <c r="H77">
         <v>1.01</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>84</v>
       </c>
       <c r="B78" t="s">
         <v>5</v>
       </c>
-      <c r="C78">
+      <c r="D78">
         <v>561</v>
       </c>
-      <c r="D78">
+      <c r="E78">
         <v>325</v>
       </c>
-      <c r="E78">
+      <c r="F78">
         <v>34</v>
       </c>
-      <c r="F78">
+      <c r="G78">
         <v>67</v>
       </c>
-      <c r="G78">
+      <c r="H78">
         <v>1.06</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>85</v>
       </c>
       <c r="B79" t="s">
         <v>10</v>
       </c>
-      <c r="C79">
+      <c r="D79">
         <v>576</v>
       </c>
-      <c r="D79">
+      <c r="E79">
         <v>400</v>
       </c>
-      <c r="E79">
+      <c r="F79">
         <v>39</v>
       </c>
-      <c r="F79">
+      <c r="G79">
         <v>61</v>
       </c>
-      <c r="G79">
+      <c r="H79">
         <v>1.07</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>86</v>
       </c>
       <c r="B80" t="s">
         <v>7</v>
       </c>
-      <c r="C80">
+      <c r="D80">
         <v>540</v>
       </c>
-      <c r="D80">
+      <c r="E80">
         <v>450</v>
       </c>
-      <c r="E80">
+      <c r="F80">
         <v>21</v>
       </c>
-      <c r="F80">
+      <c r="G80">
         <v>53</v>
       </c>
-      <c r="G80">
+      <c r="H80">
         <v>1.02</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>87</v>
       </c>
       <c r="B81" t="s">
         <v>12</v>
       </c>
-      <c r="C81">
+      <c r="D81">
         <v>545</v>
       </c>
-      <c r="D81">
+      <c r="E81">
         <v>295</v>
       </c>
-      <c r="E81">
+      <c r="F81">
         <v>28</v>
       </c>
-      <c r="F81">
+      <c r="G81">
         <v>61</v>
       </c>
-      <c r="G81">
+      <c r="H81">
         <v>1.03</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>88</v>
       </c>
       <c r="B82" t="s">
         <v>12</v>
       </c>
-      <c r="C82">
+      <c r="D82">
         <v>585</v>
       </c>
-      <c r="D82">
+      <c r="E82">
         <v>275</v>
       </c>
-      <c r="E82">
+      <c r="F82">
         <v>38</v>
       </c>
-      <c r="F82">
+      <c r="G82">
         <v>62</v>
       </c>
-      <c r="G82">
+      <c r="H82">
         <v>1.05</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>89</v>
       </c>
       <c r="B83" t="s">
         <v>12</v>
       </c>
-      <c r="C83">
+      <c r="D83">
         <v>570</v>
       </c>
-      <c r="D83">
+      <c r="E83">
         <v>280</v>
       </c>
-      <c r="E83">
+      <c r="F83">
         <v>34</v>
       </c>
-      <c r="F83">
+      <c r="G83">
         <v>61</v>
       </c>
-      <c r="G83">
+      <c r="H83">
         <v>1.04</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>90</v>
       </c>
       <c r="B84" t="s">
         <v>12</v>
       </c>
-      <c r="C84">
+      <c r="D84">
         <v>597</v>
       </c>
-      <c r="D84">
+      <c r="E84">
         <v>315</v>
       </c>
-      <c r="E84">
+      <c r="F84">
         <v>35</v>
       </c>
-      <c r="F84">
+      <c r="G84">
         <v>68</v>
       </c>
-      <c r="G84">
+      <c r="H84">
         <v>1.07</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>91</v>
       </c>
       <c r="B85" t="s">
         <v>7</v>
       </c>
-      <c r="C85">
+      <c r="D85">
         <v>530</v>
       </c>
-      <c r="D85">
+      <c r="E85">
         <v>418</v>
       </c>
-      <c r="E85">
+      <c r="F85">
         <v>17</v>
       </c>
-      <c r="F85">
+      <c r="G85">
         <v>49</v>
       </c>
-      <c r="G85">
+      <c r="H85">
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>92</v>
       </c>
       <c r="B86" t="s">
         <v>5</v>
       </c>
-      <c r="C86">
+      <c r="D86">
         <v>590</v>
       </c>
-      <c r="D86">
+      <c r="E86">
         <v>340</v>
       </c>
-      <c r="E86">
+      <c r="F86">
         <v>33</v>
       </c>
-      <c r="F86">
+      <c r="G86">
         <v>69</v>
       </c>
-      <c r="G86">
+      <c r="H86">
         <v>1.06</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>93</v>
       </c>
       <c r="B87" t="s">
         <v>5</v>
       </c>
-      <c r="C87">
+      <c r="D87">
         <v>580</v>
       </c>
-      <c r="D87">
+      <c r="E87">
         <v>317</v>
       </c>
-      <c r="E87">
+      <c r="F87">
         <v>40</v>
       </c>
-      <c r="F87">
+      <c r="G87">
         <v>64</v>
       </c>
-      <c r="G87">
+      <c r="H87">
         <v>1.07</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>94</v>
       </c>
       <c r="B88" t="s">
         <v>5</v>
       </c>
-      <c r="C88">
+      <c r="D88">
         <v>540</v>
       </c>
-      <c r="D88">
+      <c r="E88">
         <v>280</v>
       </c>
-      <c r="E88">
+      <c r="F88">
         <v>38</v>
       </c>
-      <c r="F88">
+      <c r="G88">
         <v>64</v>
       </c>
-      <c r="G88">
+      <c r="H88">
         <v>1.06</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>95</v>
       </c>
       <c r="B89" t="s">
         <v>10</v>
       </c>
-      <c r="C89">
+      <c r="D89">
         <v>600</v>
       </c>
-      <c r="D89">
+      <c r="E89">
         <v>415</v>
       </c>
-      <c r="E89">
+      <c r="F89">
         <v>45</v>
       </c>
-      <c r="F89">
+      <c r="G89">
         <v>62</v>
       </c>
-      <c r="G89">
+      <c r="H89">
         <v>1.08</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>96</v>
       </c>
       <c r="B90" t="s">
         <v>7</v>
       </c>
-      <c r="C90">
+      <c r="D90">
         <v>590</v>
       </c>
-      <c r="D90">
+      <c r="E90">
         <v>320</v>
       </c>
-      <c r="E90">
+      <c r="F90">
         <v>28</v>
       </c>
-      <c r="F90">
+      <c r="G90">
         <v>64</v>
       </c>
-      <c r="G90">
+      <c r="H90">
         <v>1.06</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>97</v>
       </c>
       <c r="B91" t="s">
         <v>5</v>
       </c>
-      <c r="C91">
+      <c r="D91">
         <v>532</v>
       </c>
-      <c r="D91">
+      <c r="E91">
         <v>268</v>
       </c>
-      <c r="E91">
+      <c r="F91">
         <v>28</v>
       </c>
-      <c r="F91">
+      <c r="G91">
         <v>59</v>
       </c>
-      <c r="G91">
+      <c r="H91">
         <v>1.04</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>98</v>
       </c>
       <c r="B92" t="s">
         <v>10</v>
       </c>
-      <c r="C92">
+      <c r="D92">
         <v>540</v>
       </c>
-      <c r="D92">
+      <c r="E92">
         <v>315</v>
       </c>
-      <c r="E92">
+      <c r="F92">
         <v>32</v>
       </c>
-      <c r="F92">
+      <c r="G92">
         <v>62</v>
       </c>
-      <c r="G92">
+      <c r="H92">
         <v>1.05</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>99</v>
       </c>
       <c r="B93" t="s">
         <v>12</v>
       </c>
-      <c r="C93">
+      <c r="D93">
         <v>564</v>
       </c>
-      <c r="D93">
+      <c r="E93">
         <v>310</v>
       </c>
-      <c r="E93">
+      <c r="F93">
         <v>36</v>
       </c>
-      <c r="F93">
+      <c r="G93">
         <v>56</v>
       </c>
-      <c r="G93">
+      <c r="H93">
         <v>1.04</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>100</v>
       </c>
       <c r="B94" t="s">
         <v>12</v>
       </c>
-      <c r="C94">
+      <c r="D94">
         <v>570</v>
       </c>
-      <c r="D94">
+      <c r="E94">
         <v>100</v>
       </c>
-      <c r="E94">
+      <c r="F94">
         <v>36</v>
       </c>
-      <c r="F94">
+      <c r="G94">
         <v>64</v>
       </c>
-      <c r="G94">
+      <c r="H94">
         <v>1.05</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>101</v>
       </c>
       <c r="B95" t="s">
         <v>5</v>
       </c>
-      <c r="C95">
+      <c r="D95">
         <v>575</v>
       </c>
-      <c r="D95">
+      <c r="E95">
         <v>100</v>
       </c>
-      <c r="E95">
+      <c r="F95">
         <v>35</v>
       </c>
-      <c r="F95">
+      <c r="G95">
         <v>69</v>
       </c>
-      <c r="G95">
+      <c r="H95">
         <v>1.06</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>102</v>
       </c>
       <c r="B96" t="s">
         <v>12</v>
       </c>
-      <c r="C96">
+      <c r="D96">
         <v>585</v>
       </c>
-      <c r="D96">
+      <c r="E96">
         <v>100</v>
       </c>
-      <c r="E96">
+      <c r="F96">
         <v>34</v>
       </c>
-      <c r="F96">
+      <c r="G96">
         <v>68</v>
       </c>
-      <c r="G96">
+      <c r="H96">
         <v>1.06</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>103</v>
       </c>
       <c r="B97" t="s">
         <v>5</v>
       </c>
-      <c r="C97">
+      <c r="D97">
         <v>560</v>
       </c>
-      <c r="D97">
+      <c r="E97">
         <v>100</v>
       </c>
-      <c r="E97">
+      <c r="F97">
         <v>33</v>
       </c>
-      <c r="F97">
+      <c r="G97">
         <v>64</v>
       </c>
-      <c r="G97">
+      <c r="H97">
         <v>1.05</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>104</v>
       </c>
       <c r="B98" t="s">
         <v>5</v>
       </c>
-      <c r="C98">
+      <c r="D98">
         <v>589</v>
       </c>
-      <c r="D98">
+      <c r="E98">
         <v>100</v>
       </c>
-      <c r="E98">
+      <c r="F98">
         <v>30</v>
       </c>
-      <c r="F98">
+      <c r="G98">
         <v>61</v>
       </c>
-      <c r="G98">
+      <c r="H98">
         <v>1.04</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>105</v>
       </c>
       <c r="B99" t="s">
         <v>16</v>
       </c>
-      <c r="C99">
+      <c r="D99">
         <v>530</v>
       </c>
-      <c r="D99">
+      <c r="E99">
         <v>348</v>
       </c>
-      <c r="E99">
+      <c r="F99">
         <v>26</v>
       </c>
-      <c r="F99">
+      <c r="G99">
         <v>57</v>
       </c>
-      <c r="G99">
+      <c r="H99">
         <v>1.03</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>106</v>
       </c>
       <c r="B100" t="s">
         <v>12</v>
       </c>
-      <c r="C100">
+      <c r="D100">
         <v>560</v>
       </c>
-      <c r="D100">
+      <c r="E100">
         <v>400</v>
       </c>
-      <c r="E100">
+      <c r="F100">
         <v>34</v>
       </c>
-      <c r="F100">
+      <c r="G100">
         <v>66</v>
       </c>
-      <c r="G100">
+      <c r="H100">
         <v>1.06</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>107</v>
       </c>
       <c r="B101" t="s">
         <v>10</v>
       </c>
-      <c r="C101">
+      <c r="D101">
         <v>520</v>
       </c>
-      <c r="D101">
+      <c r="E101">
         <v>350</v>
       </c>
-      <c r="E101">
+      <c r="F101">
         <v>28</v>
       </c>
-      <c r="F101">
+      <c r="G101">
         <v>50</v>
       </c>
-      <c r="G101">
+      <c r="H101">
         <v>1.02</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>108</v>
       </c>
       <c r="B102" t="s">
         <v>7</v>
       </c>
-      <c r="C102">
+      <c r="D102">
         <v>500</v>
       </c>
-      <c r="D102">
+      <c r="E102">
         <v>440</v>
       </c>
-      <c r="E102">
+      <c r="F102">
         <v>19</v>
       </c>
-      <c r="F102">
+      <c r="G102">
         <v>55</v>
       </c>
-      <c r="G102">
+      <c r="H102">
         <v>1.01</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>109</v>
       </c>
       <c r="B103" t="s">
         <v>5</v>
       </c>
-      <c r="C103">
+      <c r="D103">
         <v>600</v>
       </c>
-      <c r="D103">
+      <c r="E103">
         <v>0</v>
       </c>
-      <c r="E103">
+      <c r="F103">
         <v>33</v>
       </c>
-      <c r="F103">
+      <c r="G103">
         <v>60</v>
       </c>
-      <c r="G103">
+      <c r="H103">
         <v>1.05</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>110</v>
       </c>
       <c r="B104" t="s">
         <v>12</v>
       </c>
-      <c r="C104">
+      <c r="D104">
         <v>586</v>
       </c>
-      <c r="D104">
+      <c r="E104">
         <v>297</v>
       </c>
-      <c r="E104">
+      <c r="F104">
         <v>30</v>
       </c>
-      <c r="F104">
+      <c r="G104">
         <v>63</v>
       </c>
-      <c r="G104">
+      <c r="H104">
         <v>1.04</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>111</v>
       </c>
       <c r="B105" t="s">
         <v>5</v>
       </c>
-      <c r="C105">
+      <c r="D105">
         <v>540</v>
       </c>
-      <c r="D105">
+      <c r="E105">
         <v>400</v>
       </c>
-      <c r="E105">
+      <c r="F105">
         <v>34</v>
       </c>
-      <c r="F105">
+      <c r="G105">
         <v>60</v>
       </c>
-      <c r="G105">
+      <c r="H105">
         <v>1.05</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>112</v>
       </c>
       <c r="B106" t="s">
         <v>12</v>
       </c>
-      <c r="C106">
+      <c r="D106">
         <v>595</v>
       </c>
-      <c r="D106">
+      <c r="E106">
         <v>100</v>
       </c>
-      <c r="E106">
+      <c r="F106">
         <v>38</v>
       </c>
-      <c r="F106">
+      <c r="G106">
         <v>66</v>
       </c>
-      <c r="G106">
+      <c r="H106">
         <v>1.07</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>113</v>
       </c>
       <c r="B107" t="s">
         <v>5</v>
       </c>
-      <c r="C107">
+      <c r="D107">
         <v>580</v>
       </c>
-      <c r="D107">
+      <c r="E107">
         <v>330</v>
       </c>
-      <c r="E107">
+      <c r="F107">
         <v>34</v>
       </c>
-      <c r="F107">
+      <c r="G107">
         <v>62</v>
       </c>
-      <c r="G107">
+      <c r="H107">
         <v>1.06</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>114</v>
       </c>
       <c r="B108" t="s">
         <v>5</v>
       </c>
-      <c r="C108">
+      <c r="D108">
         <v>545</v>
       </c>
-      <c r="D108">
+      <c r="E108">
         <v>330</v>
       </c>
-      <c r="E108">
+      <c r="F108">
         <v>32</v>
       </c>
-      <c r="F108">
+      <c r="G108">
         <v>68</v>
       </c>
-      <c r="G108">
+      <c r="H108">
         <v>1.05</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>115</v>
       </c>
       <c r="B109" t="s">
         <v>16</v>
       </c>
-      <c r="C109">
+      <c r="D109">
         <v>532</v>
       </c>
-      <c r="D109">
+      <c r="E109">
         <v>284</v>
       </c>
-      <c r="E109">
+      <c r="F109">
         <v>26</v>
       </c>
-      <c r="F109">
+      <c r="G109">
         <v>63</v>
       </c>
-      <c r="G109">
+      <c r="H109">
         <v>1.05</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>116</v>
       </c>
       <c r="B110" t="s">
         <v>12</v>
       </c>
-      <c r="C110">
+      <c r="D110">
         <v>601</v>
       </c>
-      <c r="D110">
+      <c r="E110">
         <v>320</v>
       </c>
-      <c r="E110">
+      <c r="F110">
         <v>38</v>
       </c>
-      <c r="F110">
+      <c r="G110">
         <v>65</v>
       </c>
-      <c r="G110">
+      <c r="H110">
         <v>1.07</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>117</v>
       </c>
       <c r="B111" t="s">
         <v>10</v>
       </c>
-      <c r="C111">
+      <c r="D111">
         <v>550</v>
       </c>
-      <c r="D111">
+      <c r="E111">
         <v>340</v>
       </c>
-      <c r="E111">
+      <c r="F111">
         <v>28</v>
       </c>
-      <c r="F111">
+      <c r="G111">
         <v>49</v>
       </c>
-      <c r="G111">
+      <c r="H111">
         <v>1.02</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>118</v>
       </c>
       <c r="B112" t="s">
         <v>10</v>
       </c>
-      <c r="C112">
+      <c r="D112">
         <v>535</v>
       </c>
-      <c r="D112">
+      <c r="E112">
         <v>425</v>
       </c>
-      <c r="E112">
+      <c r="F112">
         <v>32</v>
       </c>
-      <c r="F112">
+      <c r="G112">
         <v>50</v>
       </c>
-      <c r="G112">
+      <c r="H112">
         <v>1.02</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>119</v>
       </c>
       <c r="B113" t="s">
         <v>7</v>
       </c>
-      <c r="C113">
+      <c r="D113">
         <v>525</v>
       </c>
-      <c r="D113">
+      <c r="E113">
         <v>468</v>
       </c>
-      <c r="E113">
+      <c r="F113">
         <v>23</v>
       </c>
-      <c r="F113">
+      <c r="G113">
         <v>58</v>
       </c>
-      <c r="G113">
+      <c r="H113">
         <v>1.03</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>120</v>
       </c>
       <c r="B114" t="s">
         <v>7</v>
       </c>
-      <c r="C114">
+      <c r="D114">
         <v>525</v>
       </c>
-      <c r="D114">
+      <c r="E114">
         <v>400</v>
       </c>
-      <c r="E114">
+      <c r="F114">
         <v>27</v>
       </c>
-      <c r="F114">
+      <c r="G114">
         <v>61</v>
       </c>
-      <c r="G114">
+      <c r="H114">
         <v>1.04</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>121</v>
       </c>
       <c r="B115" t="s">
         <v>7</v>
       </c>
-      <c r="C115">
+      <c r="D115">
         <v>523</v>
       </c>
-      <c r="D115">
+      <c r="E115">
         <v>480</v>
       </c>
-      <c r="E115">
+      <c r="F115">
         <v>24</v>
       </c>
-      <c r="F115">
+      <c r="G115">
         <v>54</v>
       </c>
-      <c r="G115">
+      <c r="H115">
         <v>1.02</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>122</v>
       </c>
       <c r="B116" t="s">
         <v>10</v>
       </c>
-      <c r="C116">
+      <c r="D116">
         <v>600</v>
       </c>
-      <c r="D116">
+      <c r="E116">
         <v>325</v>
       </c>
-      <c r="E116">
+      <c r="F116">
         <v>47</v>
       </c>
-      <c r="F116">
+      <c r="G116">
         <v>56</v>
       </c>
-      <c r="G116">
+      <c r="H116">
         <v>1.06</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>123</v>
       </c>
       <c r="B117" t="s">
         <v>7</v>
       </c>
-      <c r="C117">
+      <c r="D117">
         <v>532</v>
       </c>
-      <c r="D117">
+      <c r="E117">
         <v>450</v>
       </c>
-      <c r="E117">
+      <c r="F117">
         <v>20</v>
       </c>
-      <c r="F117">
+      <c r="G117">
         <v>58</v>
       </c>
-      <c r="G117">
+      <c r="H117">
         <v>1.03</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>124</v>
       </c>
       <c r="B118" t="s">
         <v>7</v>
       </c>
-      <c r="C118">
+      <c r="D118">
         <v>588</v>
       </c>
-      <c r="D118">
+      <c r="E118">
         <v>370</v>
       </c>
-      <c r="E118">
+      <c r="F118">
         <v>30</v>
       </c>
-      <c r="F118">
+      <c r="G118">
         <v>68</v>
       </c>
-      <c r="G118">
+      <c r="H118">
         <v>1.06</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>125</v>
       </c>
       <c r="B119" t="s">
         <v>10</v>
       </c>
-      <c r="C119">
+      <c r="D119">
         <v>575</v>
       </c>
-      <c r="D119">
+      <c r="E119">
         <v>300</v>
       </c>
-      <c r="E119">
+      <c r="F119">
         <v>40</v>
       </c>
-      <c r="F119">
+      <c r="G119">
         <v>55</v>
       </c>
-      <c r="G119">
+      <c r="H119">
         <v>1.05</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>126</v>
       </c>
       <c r="B120" t="s">
         <v>5</v>
       </c>
-      <c r="C120">
+      <c r="D120">
         <v>528</v>
       </c>
-      <c r="D120">
+      <c r="E120">
         <v>334</v>
       </c>
-      <c r="E120">
+      <c r="F120">
         <v>24</v>
       </c>
-      <c r="F120">
+      <c r="G120">
         <v>54</v>
       </c>
-      <c r="G120">
+      <c r="H120">
         <v>1.02</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>127</v>
       </c>
       <c r="B121" t="s">
         <v>10</v>
       </c>
-      <c r="C121">
+      <c r="D121">
         <v>560</v>
       </c>
-      <c r="D121">
+      <c r="E121">
         <v>273</v>
       </c>
-      <c r="E121">
+      <c r="F121">
         <v>28</v>
       </c>
-      <c r="F121">
+      <c r="G121">
         <v>56</v>
       </c>
-      <c r="G121">
+      <c r="H121">
         <v>1.03</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>128</v>
       </c>
       <c r="B122" t="s">
         <v>16</v>
       </c>
-      <c r="C122">
+      <c r="D122">
         <v>559</v>
       </c>
-      <c r="D122">
+      <c r="E122">
         <v>250</v>
       </c>
-      <c r="E122">
+      <c r="F122">
         <v>26</v>
       </c>
-      <c r="F122">
+      <c r="G122">
         <v>61</v>
       </c>
-      <c r="G122">
+      <c r="H122">
         <v>1.04</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>129</v>
       </c>
       <c r="B123" t="s">
         <v>12</v>
       </c>
-      <c r="C123">
+      <c r="D123">
         <v>616</v>
       </c>
-      <c r="D123">
+      <c r="E123">
         <v>281</v>
       </c>
-      <c r="E123">
+      <c r="F123">
         <v>37</v>
       </c>
-      <c r="F123">
+      <c r="G123">
         <v>68</v>
       </c>
-      <c r="G123">
+      <c r="H123">
         <v>1.07</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>130</v>
       </c>
       <c r="B124" t="s">
         <v>5</v>
       </c>
-      <c r="C124">
+      <c r="D124">
         <v>625</v>
       </c>
-      <c r="D124">
+      <c r="E124">
         <v>100</v>
       </c>
-      <c r="E124">
+      <c r="F124">
         <v>33</v>
       </c>
-      <c r="F124">
+      <c r="G124">
         <v>72</v>
       </c>
-      <c r="G124">
+      <c r="H124">
         <v>1.08</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>131</v>
       </c>
       <c r="B125" t="s">
         <v>7</v>
       </c>
-      <c r="C125">
+      <c r="D125">
         <v>534</v>
       </c>
-      <c r="D125">
+      <c r="E125">
         <v>333</v>
       </c>
-      <c r="E125">
+      <c r="F125">
         <v>21</v>
       </c>
-      <c r="F125">
+      <c r="G125">
         <v>52</v>
       </c>
-      <c r="G125">
+      <c r="H125">
         <v>1.01</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>132</v>
       </c>
       <c r="B126" t="s">
         <v>16</v>
       </c>
-      <c r="C126">
+      <c r="D126">
         <v>612</v>
       </c>
-      <c r="D126">
+      <c r="E126">
         <v>287</v>
       </c>
-      <c r="E126">
+      <c r="F126">
         <v>27</v>
       </c>
-      <c r="F126">
+      <c r="G126">
         <v>59</v>
       </c>
-      <c r="G126">
+      <c r="H126">
         <v>1.04</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>133</v>
       </c>
       <c r="B127" t="s">
         <v>12</v>
       </c>
-      <c r="C127">
+      <c r="D127">
         <v>594</v>
       </c>
-      <c r="D127">
+      <c r="E127">
         <v>271</v>
       </c>
-      <c r="E127">
+      <c r="F127">
         <v>34</v>
       </c>
-      <c r="F127">
+      <c r="G127">
         <v>66</v>
       </c>
-      <c r="G127">
+      <c r="H127">
         <v>1.06</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>134</v>
       </c>
       <c r="B128" t="s">
         <v>5</v>
       </c>
-      <c r="C128">
+      <c r="D128">
         <v>585</v>
       </c>
-      <c r="D128">
+      <c r="E128">
         <v>340</v>
       </c>
-      <c r="E128">
+      <c r="F128">
         <v>36</v>
       </c>
-      <c r="F128">
+      <c r="G128">
         <v>66</v>
       </c>
-      <c r="G128">
+      <c r="H128">
         <v>1.06</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>135</v>
       </c>
       <c r="B129" t="s">
         <v>16</v>
       </c>
-      <c r="C129">
+      <c r="D129">
         <v>530</v>
       </c>
-      <c r="D129">
+      <c r="E129">
         <v>360</v>
       </c>
-      <c r="E129">
+      <c r="F129">
         <v>27</v>
       </c>
-      <c r="F129">
+      <c r="G129">
         <v>61</v>
       </c>
-      <c r="G129">
+      <c r="H129">
         <v>1.04</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>136</v>
       </c>
       <c r="B130" t="s">
         <v>16</v>
       </c>
-      <c r="C130">
+      <c r="D130">
         <v>515</v>
       </c>
-      <c r="D130">
+      <c r="E130">
         <v>231</v>
       </c>
-      <c r="E130">
+      <c r="F130">
         <v>23</v>
       </c>
-      <c r="F130">
+      <c r="G130">
         <v>60</v>
       </c>
-      <c r="G130">
+      <c r="H130">
         <v>1.03</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>137</v>
       </c>
       <c r="B131" t="s">
         <v>7</v>
       </c>
-      <c r="C131">
+      <c r="D131">
         <v>505</v>
       </c>
-      <c r="D131">
+      <c r="E131">
         <v>490</v>
       </c>
-      <c r="E131">
+      <c r="F131">
         <v>23</v>
       </c>
-      <c r="F131">
+      <c r="G131">
         <v>52</v>
       </c>
-      <c r="G131">
+      <c r="H131">
         <v>1.01</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>138</v>
       </c>
       <c r="B132" t="s">
         <v>7</v>
       </c>
-      <c r="C132">
+      <c r="D132">
         <v>520</v>
       </c>
-      <c r="D132">
+      <c r="E132">
         <v>469</v>
       </c>
-      <c r="E132">
+      <c r="F132">
         <v>22</v>
       </c>
-      <c r="F132">
+      <c r="G132">
         <v>55</v>
       </c>
-      <c r="G132">
+      <c r="H132">
         <v>1.02</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>139</v>
       </c>
       <c r="B133" t="s">
         <v>12</v>
       </c>
-      <c r="C133">
+      <c r="D133">
         <v>585</v>
       </c>
-      <c r="D133">
+      <c r="E133">
         <v>295</v>
       </c>
-      <c r="E133">
+      <c r="F133">
         <v>34</v>
       </c>
-      <c r="F133">
+      <c r="G133">
         <v>64</v>
       </c>
-      <c r="G133">
+      <c r="H133">
         <v>1.05</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>140</v>
       </c>
       <c r="B134" t="s">
         <v>7</v>
       </c>
-      <c r="C134">
+      <c r="D134">
         <v>530</v>
       </c>
-      <c r="D134">
+      <c r="E134">
         <v>405</v>
       </c>
-      <c r="E134">
+      <c r="F134">
         <v>23</v>
       </c>
-      <c r="F134">
+      <c r="G134">
         <v>53</v>
       </c>
-      <c r="G134">
+      <c r="H134">
         <v>1.02</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>141</v>
       </c>
       <c r="B135" t="s">
         <v>7</v>
       </c>
-      <c r="C135">
+      <c r="D135">
         <v>537</v>
       </c>
-      <c r="D135">
+      <c r="E135">
         <v>100</v>
       </c>
-      <c r="E135">
+      <c r="F135">
         <v>23</v>
       </c>
-      <c r="F135">
+      <c r="G135">
         <v>55</v>
       </c>
-      <c r="G135">
+      <c r="H135">
         <v>1.02</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>142</v>
       </c>
       <c r="B136" t="s">
         <v>5</v>
       </c>
-      <c r="C136">
+      <c r="D136">
         <v>580</v>
       </c>
-      <c r="D136">
+      <c r="E136">
         <v>350</v>
       </c>
-      <c r="E136">
+      <c r="F136">
         <v>35</v>
       </c>
-      <c r="F136">
+      <c r="G136">
         <v>60</v>
       </c>
-      <c r="G136">
+      <c r="H136">
         <v>1.05</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>143</v>
       </c>
       <c r="B137" t="s">
         <v>12</v>
       </c>
-      <c r="C137">
+      <c r="D137">
         <v>550</v>
       </c>
-      <c r="D137">
+      <c r="E137">
         <v>280</v>
       </c>
-      <c r="E137">
+      <c r="F137">
         <v>33</v>
       </c>
-      <c r="F137">
+      <c r="G137">
         <v>62</v>
       </c>
-      <c r="G137">
+      <c r="H137">
         <v>1.05</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>144</v>
       </c>
       <c r="B138" t="s">
         <v>5</v>
       </c>
-      <c r="C138">
+      <c r="D138">
         <v>540</v>
       </c>
-      <c r="D138">
+      <c r="E138">
         <v>300</v>
       </c>
-      <c r="E138">
+      <c r="F138">
         <v>31</v>
       </c>
-      <c r="F138">
+      <c r="G138">
         <v>68</v>
       </c>
-      <c r="G138">
+      <c r="H138">
         <v>1.06</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>145</v>
       </c>
       <c r="B139" t="s">
         <v>16</v>
       </c>
-      <c r="C139">
+      <c r="D139">
         <v>590</v>
       </c>
-      <c r="D139">
+      <c r="E139">
         <v>340</v>
       </c>
-      <c r="E139">
+      <c r="F139">
         <v>25</v>
       </c>
-      <c r="F139">
+      <c r="G139">
         <v>60</v>
       </c>
-      <c r="G139">
+      <c r="H139">
         <v>1.05</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>146</v>
       </c>
       <c r="B140" t="s">
         <v>7</v>
       </c>
-      <c r="C140">
+      <c r="D140">
         <v>526</v>
       </c>
-      <c r="D140">
+      <c r="E140">
         <v>480</v>
       </c>
-      <c r="E140">
+      <c r="F140">
         <v>21</v>
       </c>
-      <c r="F140">
+      <c r="G140">
         <v>55</v>
       </c>
-      <c r="G140">
+      <c r="H140">
         <v>1.02</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>147</v>
       </c>
       <c r="B141" t="s">
         <v>12</v>
       </c>
-      <c r="C141">
+      <c r="D141">
         <v>590</v>
       </c>
-      <c r="D141">
+      <c r="E141">
         <v>273</v>
       </c>
-      <c r="E141">
+      <c r="F141">
         <v>35</v>
       </c>
-      <c r="F141">
+      <c r="G141">
         <v>66</v>
       </c>
-      <c r="G141">
+      <c r="H141">
         <v>1.06</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>148</v>
       </c>
       <c r="B142" t="s">
         <v>7</v>
       </c>
-      <c r="C142">
+      <c r="D142">
         <v>490</v>
       </c>
-      <c r="D142">
+      <c r="E142">
         <v>100</v>
       </c>
-      <c r="E142">
+      <c r="F142">
         <v>30</v>
       </c>
-      <c r="F142">
+      <c r="G142">
         <v>60</v>
       </c>
-      <c r="G142">
+      <c r="H142">
         <v>1.04</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>149</v>
       </c>
       <c r="B143" t="s">
         <v>7</v>
       </c>
-      <c r="C143">
+      <c r="D143">
         <v>550</v>
       </c>
-      <c r="D143">
+      <c r="E143">
         <v>100</v>
       </c>
-      <c r="E143">
+      <c r="F143">
         <v>28</v>
       </c>
-      <c r="F143">
+      <c r="G143">
         <v>60</v>
       </c>
-      <c r="G143">
+      <c r="H143">
         <v>1.04</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>150</v>
       </c>
       <c r="B144" t="s">
         <v>5</v>
       </c>
-      <c r="C144">
+      <c r="D144">
         <v>580</v>
       </c>
-      <c r="D144">
+      <c r="E144">
         <v>300</v>
       </c>
-      <c r="E144">
+      <c r="F144">
         <v>39</v>
       </c>
-      <c r="F144">
+      <c r="G144">
         <v>62</v>
       </c>
-      <c r="G144">
+      <c r="H144">
         <v>1.06</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>151</v>
       </c>
       <c r="B145" t="s">
         <v>10</v>
       </c>
-      <c r="C145">
+      <c r="D145">
         <v>500</v>
       </c>
-      <c r="D145">
+      <c r="E145">
         <v>400</v>
       </c>
-      <c r="E145">
+      <c r="F145">
         <v>25</v>
       </c>
-      <c r="F145">
+      <c r="G145">
         <v>55</v>
       </c>
-      <c r="G145">
+      <c r="H145">
         <v>1.02</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>152</v>
       </c>
       <c r="B146" t="s">
         <v>12</v>
       </c>
-      <c r="C146">
+      <c r="D146">
         <v>615</v>
       </c>
-      <c r="D146">
+      <c r="E146">
         <v>0</v>
       </c>
-      <c r="E146">
+      <c r="F146">
         <v>33</v>
       </c>
-      <c r="F146">
+      <c r="G146">
         <v>60</v>
       </c>
-      <c r="G146">
+      <c r="H146">
         <v>1.06</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>153</v>
       </c>
       <c r="B147" t="s">
         <v>7</v>
       </c>
-      <c r="C147">
+      <c r="D147">
         <v>585</v>
       </c>
-      <c r="D147">
+      <c r="E147">
         <v>200</v>
       </c>
-      <c r="E147">
+      <c r="F147">
         <v>32</v>
       </c>
-      <c r="F147">
+      <c r="G147">
         <v>63</v>
       </c>
-      <c r="G147">
+      <c r="H147">
         <v>1.05</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>154</v>
       </c>
       <c r="B148" t="s">
         <v>7</v>
       </c>
-      <c r="C148">
+      <c r="D148">
         <v>536</v>
       </c>
-      <c r="D148">
+      <c r="E148">
         <v>480</v>
       </c>
-      <c r="E148">
+      <c r="F148">
         <v>21</v>
       </c>
-      <c r="F148">
+      <c r="G148">
         <v>54</v>
       </c>
-      <c r="G148">
+      <c r="H148">
         <v>1.02</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>155</v>
       </c>
       <c r="B149" t="s">
         <v>10</v>
       </c>
-      <c r="C149">
+      <c r="D149">
         <v>504</v>
       </c>
-      <c r="D149">
+      <c r="E149">
         <v>452</v>
       </c>
-      <c r="E149">
+      <c r="F149">
         <v>22</v>
       </c>
-      <c r="F149">
+      <c r="G149">
         <v>51</v>
       </c>
-      <c r="G149">
+      <c r="H149">
         <v>1.01</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>156</v>
       </c>
       <c r="B150" t="s">
         <v>7</v>
       </c>
-      <c r="C150">
+      <c r="D150">
         <v>560</v>
       </c>
-      <c r="D150">
+      <c r="E150">
         <v>425</v>
       </c>
-      <c r="E150">
+      <c r="F150">
         <v>20</v>
       </c>
-      <c r="F150">
+      <c r="G150">
         <v>58</v>
       </c>
-      <c r="G150">
+      <c r="H150">
         <v>1.02</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>157</v>
       </c>
       <c r="B151" t="s">
         <v>10</v>
       </c>
-      <c r="C151">
+      <c r="D151">
         <v>504</v>
       </c>
-      <c r="D151">
+      <c r="E151">
         <v>418</v>
       </c>
-      <c r="E151">
+      <c r="F151">
         <v>29</v>
       </c>
-      <c r="F151">
+      <c r="G151">
         <v>53</v>
       </c>
-      <c r="G151">
+      <c r="H151">
         <v>1.02</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Convert numeric words to numbers
</commit_message>
<xml_diff>
--- a/champions.xlsx
+++ b/champions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\5dars\PycharmProjects\Data Cleaning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B8C240-61DC-44F0-A9F1-9BEE1FAC8114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31ED8AB0-E12F-46A3-B062-083F3CB93CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A8605B52-9432-49E7-A343-C706373D400E}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="162">
   <si>
     <t>Champion Name</t>
   </si>
@@ -503,6 +503,9 @@
   </si>
   <si>
     <t xml:space="preserve">                      Base Health</t>
+  </si>
+  <si>
+    <t>twenty one</t>
   </si>
 </sst>
 </file>
@@ -1366,7 +1369,7 @@
   <dimension ref="A1:H151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1463,8 +1466,8 @@
       <c r="E4">
         <v>418</v>
       </c>
-      <c r="F4">
-        <v>21</v>
+      <c r="F4" t="s">
+        <v>161</v>
       </c>
       <c r="G4">
         <v>53</v>

</xml_diff>